<commit_message>
Enabled macros to calculate turns taken
</commit_message>
<xml_diff>
--- a/Testing balance.xlsx
+++ b/Testing balance.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shahidh7\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humza_000\Documents\GitHub\ALL Project 2TheCivilWarOfMalibu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +23,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Humza Shahid</author>
+  </authors>
+  <commentList>
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{98607936-B4BA-46AF-A794-B3E9C060CF14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Humza Shahid:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assuming both attack and defense values are standard and that both armies only choose to attack.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{82E5E670-A899-4DB9-9824-FED8C3D2547A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Humza Shahid:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assuming both attack and defense values are standard and that both armies only choose to attack.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Troops</t>
   </si>
@@ -83,20 +141,26 @@
     <t>Outcome</t>
   </si>
   <si>
-    <t>Possibility</t>
-  </si>
-  <si>
     <t>Std Atk</t>
   </si>
   <si>
     <t>Std Def</t>
+  </si>
+  <si>
+    <t>Outcome type</t>
+  </si>
+  <si>
+    <t>Turns for army 1 to defeat army 2</t>
+  </si>
+  <si>
+    <t>Turns for army 2 to defeat army 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +193,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -156,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -352,19 +429,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -375,15 +439,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -412,23 +467,49 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -437,81 +518,22 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -521,156 +543,113 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -952,430 +931,427 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="2" style="25" customWidth="1"/>
     <col min="11" max="16" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="K3" s="7" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="K3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="28" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="11"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="36"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>60</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="13">
         <v>10</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="29">
+      <c r="E5" s="2">
         <v>90</v>
       </c>
-      <c r="G5" s="20">
+      <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="39"/>
+      <c r="K5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="19"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>25</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="13">
         <v>10</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="29">
+      <c r="E6" s="2">
         <v>20</v>
       </c>
-      <c r="G6" s="20">
+      <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="K6" s="45"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="39"/>
+      <c r="K6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="19"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>10</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="13">
         <v>9</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="29">
+      <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="G7" s="20">
+      <c r="F7" s="11">
         <v>4</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="39"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="30"/>
     </row>
-    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="8">
         <v>100</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="14">
         <v>10</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="30">
+      <c r="E8" s="8">
         <v>40</v>
       </c>
-      <c r="G8" s="18">
+      <c r="F8" s="9">
         <v>5</v>
       </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="42"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="35"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="K13" s="7" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="K13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="9"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="24"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="27" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="K14" s="47" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="36"/>
+      <c r="K14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="51" t="s">
+      <c r="L14" s="32"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="52"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="36"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="str">
+      <c r="B15" s="15" t="str">
         <f>B5</f>
         <v>HoloTank</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="22">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18">
         <v>1</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="K15" s="12" t="str">
+      <c r="F15" s="16"/>
+      <c r="G15" s="19"/>
+      <c r="K15" s="15" t="str">
         <f>B5</f>
         <v>HoloTank</v>
       </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="36">
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18">
         <v>1</v>
       </c>
-      <c r="P15" s="37"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="19"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="str">
+      <c r="B16" s="15" t="str">
         <f t="shared" ref="B16:B18" si="0">B6</f>
         <v>HoloBike</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="22">
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18">
         <v>1</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="K16" s="12" t="str">
+      <c r="F16" s="16"/>
+      <c r="G16" s="19"/>
+      <c r="K16" s="15" t="str">
         <f t="shared" ref="K16:K18" si="1">B6</f>
         <v>HoloBike</v>
       </c>
-      <c r="L16" s="21"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="22">
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18">
         <v>1</v>
       </c>
-      <c r="P16" s="13"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="19"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="str">
+      <c r="B17" s="15" t="str">
         <f t="shared" si="0"/>
         <v>HoloSoldier</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="22">
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18">
         <v>1</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="K17" s="12" t="str">
+      <c r="F17" s="16"/>
+      <c r="G17" s="19"/>
+      <c r="K17" s="15" t="str">
         <f t="shared" si="1"/>
         <v>HoloSoldier</v>
       </c>
-      <c r="L17" s="21"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="22">
+      <c r="L17" s="16"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="18">
         <v>1</v>
       </c>
-      <c r="P17" s="13"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="19"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="str">
+      <c r="B18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>HoloXcom</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="22">
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18">
         <v>1</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="K18" s="12" t="str">
+      <c r="F18" s="16"/>
+      <c r="G18" s="19"/>
+      <c r="K18" s="15" t="str">
         <f t="shared" si="1"/>
         <v>HoloXcom</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="22">
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18">
         <v>1</v>
       </c>
-      <c r="P18" s="13"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="19"/>
     </row>
     <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="G19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="N19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="3" t="s">
+      <c r="O19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P19" s="15" t="s">
+      <c r="P19" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="16">
-        <f>((C5-D5)*F15)+((C6-D6)*F16)+((C7-D7)*F17)+((C8-D8)*F18)</f>
+      <c r="B20" s="7">
+        <f>((C5-D5)*E15)+((C6-D6)*E16)+((C7-D7)*E17)+((C8-D8)*E18)</f>
         <v>156</v>
       </c>
-      <c r="C20" s="17">
-        <f>(C5*F15)+(C6*F16)+(C7*F17)+(C8+F18)</f>
-        <v>196</v>
-      </c>
-      <c r="D20" s="17">
-        <f>((C5+D5)*F15)+((C6+D6)*F16)+((C7+D7)*F17)+((C8+D8)*F18)</f>
+      <c r="C20" s="8">
+        <f>(C5*E15)+(C6*E16)+(C7*E17)+(C8*E18)</f>
+        <v>195</v>
+      </c>
+      <c r="D20" s="8">
+        <f>((C5+D5)*E15)+((C6+D6)*E16)+((C7+D7)*E17)+((C8+D8)*E18)</f>
         <v>234</v>
       </c>
-      <c r="E20" s="17">
-        <f>((F5-G5)*F15)+((F6-G6)*F16)+((F7-G7)*F17)+((F8-G8)*F18)</f>
+      <c r="E20" s="8">
+        <f>((E5-F5)*E15)+((E6-F6)*E16)+((E7-F7)*E17)+((E8-F8)*E18)</f>
         <v>136</v>
       </c>
-      <c r="F20" s="17">
-        <f>(F5*F15)+(F6*F16)+(F7*F17)+(F8*F18)</f>
+      <c r="F20" s="8">
+        <f>(E5*E15)+(E6*E16)+(E7*E17)+(E8*E18)</f>
         <v>155</v>
       </c>
-      <c r="G20" s="18">
-        <f>((F5+G5)*F15)+((F6+G6)*F16)+((F7+G7)*F17)+((F8+G8)*F18)</f>
+      <c r="G20" s="9">
+        <f>((E5+F5)*E15)+((E6+F6)*E16)+((E7+F7)*E17)+((E8+F8)*E18)</f>
         <v>174</v>
       </c>
-      <c r="K20" s="16">
-        <f>((C5-D5)*O15)+((C6-D6)*O16)+((C7-D7)*O17)+((C8-D8)*O18)</f>
+      <c r="K20" s="7">
+        <f>((C5-D5)*N15)+((C6-D6)*N16)+((C7-D7)*N17)+((C8-D8)*N18)</f>
         <v>156</v>
       </c>
-      <c r="L20" s="17">
-        <f>(C5*O15)+(C6*O16)+(C7*O17)+(C8*O18)</f>
+      <c r="L20" s="8">
+        <f>(C5*N15)+(C6*N16)+(C7*N17)+(C8*N18)</f>
         <v>195</v>
       </c>
-      <c r="M20" s="17">
-        <f>((C5+D5)*O15)+((C6+D6)*O16)+((C7+D7)*O17)+((C8+D8)*O18)</f>
+      <c r="M20" s="8">
+        <f>((C5+D5)*N15)+((C6+D6)*N16)+((C7+D7)*N17)+((C8+D8)*N18)</f>
         <v>234</v>
       </c>
-      <c r="N20" s="17">
-        <f>((F5-G5)*O15)+((F6-G6)*O16)+((F7-G7)*O17)+((F8-G8)*O18)</f>
+      <c r="N20" s="8">
+        <f>((E5-F5)*N15)+((E6-F6)*N16)+((E7-F7)*N17)+((E8-F8)*N18)</f>
         <v>136</v>
       </c>
-      <c r="O20" s="17">
-        <f>(F5*O15)+(F6*O16)+(F7*O17)+(F8*O18)</f>
+      <c r="O20" s="8">
+        <f>(E5*N15)+(E6*N16)+(E7*N17)+(E8*N18)</f>
         <v>155</v>
       </c>
-      <c r="P20" s="18">
-        <f>((F5+G5)*O15)+((F6+G6)*O16)+((F7+G7)*O17)+((F8+G8)*O18)</f>
+      <c r="P20" s="9">
+        <f>((E5+F5)*N15)+((E6+F6)*N16)+((E7+F7)*N17)+((E8+F8)*N18)</f>
         <v>174</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="33">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="H1:J1048576"/>
+    <mergeCell ref="K4:M4"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="K8:M8"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="N5:P5"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="H1:J1048576"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>